<commit_message>
update appendix B text
</commit_message>
<xml_diff>
--- a/tables/CIIP_phase2_scenarios.xlsx
+++ b/tables/CIIP_phase2_scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\docs\CDM-manual\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthipsey/AED Dropbox/Matt Hipsey/GitHub/cdm-science/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AFD1C3-DDCA-490D-9FC7-4582FD682676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D364534F-8824-5849-B80C-013C8033F084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5055" yWindow="2490" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5060" yWindow="2500" windowWidth="21600" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>Ik</t>
   </si>
   <si>
-    <t>CIIP phase 1</t>
-  </si>
-  <si>
     <t>Fsed_amm</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>0.68 ± 0.41</t>
+  </si>
+  <si>
+    <t>GEN 0 (CIIP phase 1)</t>
   </si>
 </sst>
 </file>
@@ -600,39 +600,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -650,15 +650,15 @@
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="D2" s="2">
         <v>0.2</v>
@@ -691,15 +691,15 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2">
         <v>0.4</v>
@@ -732,15 +732,15 @@
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
@@ -773,15 +773,15 @@
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
         <v>7.5</v>
@@ -814,15 +814,15 @@
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2">
         <v>9</v>
@@ -855,15 +855,15 @@
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -881,15 +881,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -907,15 +907,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2">
         <v>0.3</v>
@@ -933,15 +933,15 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2">
         <v>0.375</v>
@@ -959,15 +959,15 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2">
         <v>0.3</v>
@@ -985,15 +985,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="D12" s="2">
         <v>0.05</v>
@@ -1011,15 +1011,15 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="2">
         <v>0.2</v>
@@ -1037,15 +1037,15 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2">
         <v>0.1</v>
@@ -1063,15 +1063,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2">
         <v>0.1875</v>
@@ -1089,15 +1089,15 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2">
         <v>0.375</v>
@@ -1115,15 +1115,15 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="D17" s="2">
         <v>-15</v>
@@ -1141,15 +1141,15 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="2">
         <v>-15</v>
@@ -1167,15 +1167,15 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2">
         <v>-30</v>
@@ -1193,15 +1193,15 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="2">
         <v>-30</v>
@@ -1219,15 +1219,15 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="2">
         <v>-30</v>
@@ -1260,12 +1260,12 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1284,7 +1284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1440,193 +1440,193 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A703BD-64DF-4D56-BF20-6C7925813422}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="F2" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="F7" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="E9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>